<commit_message>
update on 14 March
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bikash/TEA-cook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00-Bikash\01-cooking\01-analysis-files\TEA-cook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB108AF-F4B4-1A4D-8F2F-295577CA3844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B815A2D9-A6A2-49B1-855D-02585EB27FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{CE22EA52-FFF3-A042-B963-1F0F7F7741CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE22EA52-FFF3-A042-B963-1F0F7F7741CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -258,9 +247,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;₹&quot;* #,##0.00_);_(&quot;₹&quot;* \(#,##0.00\);_(&quot;₹&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;₹&quot;* #,##0.00_);_(&quot;₹&quot;* \(#,##0.00\);_(&quot;₹&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -754,7 +743,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -821,10 +810,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -833,10 +822,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -863,10 +852,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -887,10 +876,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -914,7 +903,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{DB3FAB90-6D26-41F5-B68B-443C652ED851}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -927,7 +918,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1215,7 +1206,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1225,13 +1216,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E965585B-0816-7C47-9CA5-272A95E3A4DA}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:B31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="25.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1257,7 +1248,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -1268,7 +1259,7 @@
       <c r="D3" s="13"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
@@ -1279,7 +1270,7 @@
       <c r="D4" s="18"/>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
@@ -1293,7 +1284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1307,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
@@ -1321,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
@@ -1341,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
@@ -1350,7 +1341,7 @@
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
     </row>
-    <row r="10" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
@@ -1364,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>20</v>
       </c>
@@ -1378,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>22</v>
       </c>
@@ -1398,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>24</v>
       </c>
@@ -1418,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>26</v>
       </c>
@@ -1427,7 +1418,7 @@
       <c r="D14" s="30"/>
       <c r="E14" s="31"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>27</v>
       </c>
@@ -1441,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>29</v>
       </c>
@@ -1461,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>30</v>
       </c>
@@ -1475,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>16</v>
       </c>
@@ -1495,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="38" t="s">
         <v>31</v>
       </c>
@@ -1504,7 +1495,7 @@
       <c r="D19" s="30"/>
       <c r="E19" s="31"/>
     </row>
-    <row r="20" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>32</v>
       </c>
@@ -1515,7 +1506,7 @@
       <c r="D20" s="39"/>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>33</v>
       </c>
@@ -1529,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>34</v>
       </c>
@@ -1543,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>36</v>
       </c>
@@ -1557,7 +1548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>38</v>
       </c>
@@ -1577,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>39</v>
       </c>
@@ -1588,7 +1579,7 @@
       <c r="D25" s="40"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="24" t="s">
         <v>41</v>
       </c>
@@ -1602,7 +1593,7 @@
       </c>
       <c r="E26" s="27"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="35" t="s">
         <v>42</v>
       </c>
@@ -1611,7 +1602,7 @@
       <c r="D27" s="30"/>
       <c r="E27" s="31"/>
     </row>
-    <row r="28" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>43</v>
       </c>
@@ -1622,7 +1613,7 @@
       <c r="D28" s="39"/>
       <c r="E28" s="14"/>
     </row>
-    <row r="29" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>45</v>
       </c>
@@ -1642,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>46</v>
       </c>
@@ -1653,7 +1644,7 @@
       <c r="D30" s="40"/>
       <c r="E30" s="19"/>
     </row>
-    <row r="31" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="47" t="s">
         <v>47</v>
       </c>
@@ -1667,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>